<commit_message>
Facta View - SetTitle : Change to reference last month Added: Facta View - Print Month Contracts
</commit_message>
<xml_diff>
--- a/TemplateFacta.xlsx
+++ b/TemplateFacta.xlsx
@@ -443,20 +443,20 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="5"/>
-    <col min="2" max="2" width="20.140625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="76.7109375" style="6" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" style="6" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" style="6" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="68" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" style="6" customWidth="1"/>
+    <col min="8" max="8" width="22.7109375" style="6" customWidth="1"/>
     <col min="9" max="9" width="12.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="4"/>
   </cols>

</xml_diff>